<commit_message>
fix bug and validate Staff Form
</commit_message>
<xml_diff>
--- a/excels/Staff.xlsx
+++ b/excels/Staff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\FastFoodStore\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4Code\Java\FastFoodStore\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29AAE48-DEA5-4224-AA8B-8D1B1900F799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7C1BC7-91DA-4ACB-AB43-B58D2F95849F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2880" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff_M" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -113,18 +113,6 @@
   </si>
   <si>
     <t>Crew</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>Quận 1</t>
-  </si>
-  <si>
-    <t>2003-30-10</t>
   </si>
 </sst>
 </file>
@@ -496,21 +484,21 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -556,7 +544,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -579,7 +567,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -602,7 +590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -625,7 +613,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -648,33 +636,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>6999</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7">
-        <v>363855850</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1" xr:uid="{794DE7E2-FA69-479F-9FE9-8E9514856C57}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>